<commit_message>
ESR work - lots of mess!
</commit_message>
<xml_diff>
--- a/apps/ESR_guilds/EBS_2022_cpue_sum.xlsx
+++ b/apps/ESR_guilds/EBS_2022_cpue_sum.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kerim.aydin\Work\src\reem_diets\apps\ESR_guilds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C80529D9-59D9-40CE-9934-59AFC442775C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42975867-F240-430D-A18A-10D2631399CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="guild_bio_2024test" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2305,16 +2305,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>319086</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>157161</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>42861</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>42861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2638,11 +2638,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>